<commit_message>
Se incorporan los dos test restantes y modificaciones varias
</commit_message>
<xml_diff>
--- a/Documentacion_tests/Documentacion_tests.xlsx
+++ b/Documentacion_tests/Documentacion_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Downloads\ProyectoMundial\Documentacion_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FB9E19-0898-4A6A-AF73-1F0B2F0DAB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAF14AE-8C4C-4987-B556-FC9EBF19ACF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{81273898-7740-41E9-88A4-AB9C2233E968}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Test Case #</t>
   </si>
@@ -72,6 +72,38 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Chequear si se puede crear un post correctamente</t>
+  </si>
+  <si>
+    <t>titulo=random
+equipo=random
+posteo="Esta es una prueba 1234567890 /&amp;%#$"
+autor_prueba=User.objects.create(id=1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El posteo se debe crear correctamente </t>
+  </si>
+  <si>
+    <t>El posteo se creó en el blog correctamente</t>
+  </si>
+  <si>
+    <t>Corroborar si toma como válido el registro de usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'last_name': 'Ronaldo',
+'first_name': 'Cristiano',
+'username': 'cronaldo7',
+'email':'cronaldo7@example.com',
+'password1': 'Portugal123',
+'password2': 'Portugal123'</t>
+  </si>
+  <si>
+    <t>El registro debe ser válido</t>
+  </si>
+  <si>
+    <t>El registro fue válido</t>
   </si>
 </sst>
 </file>
@@ -136,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -146,6 +178,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,14 +499,14 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.1796875" customWidth="1"/>
     <col min="2" max="2" width="30.36328125" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="3" max="3" width="42.36328125" customWidth="1"/>
     <col min="4" max="4" width="20.36328125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="11.26953125" customWidth="1"/>
@@ -517,25 +552,45 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>